<commit_message>
Product script also done now both working main category then subcategory and the products
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
-  <si>
-    <t>S #</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
   <si>
     <t>Code</t>
   </si>
@@ -81,9 +75,6 @@
     <t>Ev-01-009</t>
   </si>
   <si>
-    <t>Varifocal Portable Otoscope Ophthalmoscope Ophthalmoskop</t>
-  </si>
-  <si>
     <t>Ev-01-010</t>
   </si>
   <si>
@@ -196,6 +187,42 @@
   </si>
   <si>
     <t>Buck Percussion Hammers</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Varifocal Portable Otoscope Ophthalmoscope</t>
+  </si>
+  <si>
+    <t>Anesthesia Instruments</t>
+  </si>
+  <si>
+    <t>Ev-02-028</t>
+  </si>
+  <si>
+    <t>Suction Tube Poole</t>
+  </si>
+  <si>
+    <t>10mm (30 Charr.)</t>
+  </si>
+  <si>
+    <t>Ev-02-029</t>
+  </si>
+  <si>
+    <t>6mm (18 Charr.)</t>
+  </si>
+  <si>
+    <t>Ev-02-030</t>
+  </si>
+  <si>
+    <t>8mm (23 Charr.)</t>
+  </si>
+  <si>
+    <t>Ev-02-031</t>
+  </si>
+  <si>
+    <t>Suction Tube Yankauer</t>
   </si>
 </sst>
 </file>
@@ -230,12 +257,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7B7B7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -271,12 +304,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,453 +592,451 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="C19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>